<commit_message>
finally got lower mse in optimised model for bundesliga see bundeswithprevseas.R
</commit_message>
<xml_diff>
--- a/buli2122.xlsx
+++ b/buli2122.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idrishedayat/Documents/STAT0035/DissertationOfficial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC5BEBB2-D777-8048-A164-450F8EE4305C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3972816-E33C-FB42-9C6F-B7265970D98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15260"/>
+    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15780"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -1262,7 +1262,7 @@
   <dimension ref="A1:N307"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N91" sqref="N91"/>
+      <selection activeCell="I325" sqref="I325"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1662,7 +1662,7 @@
       </c>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -10703,13 +10703,13 @@
         <v>25</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>52</v>
+        <v>113</v>
       </c>
       <c r="C226" s="4">
         <v>44626</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="E226" s="3" t="s">
         <v>53</v>

</xml_diff>